<commit_message>
update apps metadata plus:
update logcat filters,
update experiment run time estimates,
add adb help printout
</commit_message>
<xml_diff>
--- a/resources/run_time_estimates.xlsx
+++ b/resources/run_time_estimates.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="16828"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="17426"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650"/>
@@ -500,7 +500,7 @@
   <dimension ref="B2:K28"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D26" sqref="D26"/>
+      <selection activeCell="B17" sqref="B17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -594,7 +594,7 @@
     </row>
     <row r="7" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B7" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C7" s="1">
         <v>4</v>
@@ -604,23 +604,23 @@
       </c>
       <c r="E7" s="2">
         <f t="shared" si="0"/>
-        <v>8.6920000000000002</v>
+        <v>8.2680000000000007</v>
       </c>
       <c r="F7" s="2">
         <f t="shared" si="1"/>
-        <v>0.96577777777777785</v>
+        <v>0.91866666666666674</v>
       </c>
       <c r="G7" s="5">
         <f t="shared" si="2"/>
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H7" s="2">
         <f t="shared" si="3"/>
-        <v>8.6920000000000002</v>
+        <v>8.2680000000000007</v>
       </c>
       <c r="I7" s="2">
         <f t="shared" si="4"/>
-        <v>0.96577777777777785</v>
+        <v>0.91866666666666674</v>
       </c>
       <c r="J7" s="5">
         <f t="shared" si="5"/>
@@ -670,33 +670,33 @@
     </row>
     <row r="9" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B9" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C9" s="1">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="D9" s="1">
         <v>3</v>
       </c>
       <c r="E9" s="2">
         <f t="shared" si="0"/>
-        <v>26.076000000000004</v>
+        <v>26.871000000000002</v>
       </c>
       <c r="F9" s="2">
         <f t="shared" si="1"/>
-        <v>2.897333333333334</v>
+        <v>2.9856666666666669</v>
       </c>
       <c r="G9" s="5">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H9" s="2">
         <f t="shared" si="3"/>
-        <v>8.6920000000000002</v>
+        <v>8.956999999999999</v>
       </c>
       <c r="I9" s="2">
         <f t="shared" si="4"/>
-        <v>0.96577777777777785</v>
+        <v>0.99522222222222212</v>
       </c>
       <c r="J9" s="5">
         <f t="shared" si="5"/>
@@ -746,7 +746,7 @@
     </row>
     <row r="11" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B11" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C11" s="1">
         <v>60</v>
@@ -756,23 +756,23 @@
       </c>
       <c r="E11" s="2">
         <f t="shared" si="0"/>
-        <v>130.38</v>
+        <v>124.02000000000001</v>
       </c>
       <c r="F11" s="2">
         <f t="shared" si="1"/>
-        <v>14.486666666666666</v>
+        <v>13.780000000000001</v>
       </c>
       <c r="G11" s="5">
         <f t="shared" si="2"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H11" s="2">
         <f t="shared" si="3"/>
-        <v>43.46</v>
+        <v>41.34</v>
       </c>
       <c r="I11" s="2">
         <f t="shared" si="4"/>
-        <v>4.8288888888888888</v>
+        <v>4.5933333333333337</v>
       </c>
       <c r="J11" s="5">
         <f t="shared" si="5"/>
@@ -833,7 +833,7 @@
     </row>
     <row r="14" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B14" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C14" s="1">
         <v>60</v>
@@ -843,27 +843,27 @@
       </c>
       <c r="E14" s="2">
         <f t="shared" si="6"/>
-        <v>130.38</v>
+        <v>124.02000000000001</v>
       </c>
       <c r="F14" s="2">
         <f t="shared" si="7"/>
-        <v>14.486666666666666</v>
+        <v>13.780000000000001</v>
       </c>
       <c r="G14" s="5">
         <f t="shared" si="8"/>
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H14" s="2">
         <f t="shared" si="9"/>
-        <v>130.38</v>
+        <v>124.02000000000001</v>
       </c>
       <c r="I14" s="2">
         <f t="shared" si="10"/>
-        <v>14.486666666666666</v>
+        <v>13.780000000000001</v>
       </c>
       <c r="J14" s="5">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="15" spans="2:11" x14ac:dyDescent="0.35">
@@ -903,7 +903,7 @@
     </row>
     <row r="16" spans="2:11" x14ac:dyDescent="0.35">
       <c r="B16" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C16" s="1">
         <v>120</v>
@@ -913,27 +913,27 @@
       </c>
       <c r="E16" s="2">
         <f t="shared" si="6"/>
-        <v>260.76</v>
+        <v>248.04000000000002</v>
       </c>
       <c r="F16" s="2">
         <f t="shared" si="7"/>
-        <v>28.973333333333333</v>
+        <v>27.560000000000002</v>
       </c>
       <c r="G16" s="5">
         <f t="shared" si="8"/>
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="H16" s="2">
         <f t="shared" si="9"/>
-        <v>260.76</v>
+        <v>248.04000000000002</v>
       </c>
       <c r="I16" s="2">
         <f t="shared" si="10"/>
-        <v>28.973333333333333</v>
+        <v>27.560000000000002</v>
       </c>
       <c r="J16" s="5">
         <f t="shared" si="11"/>
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="17" spans="2:10" x14ac:dyDescent="0.35">
@@ -973,7 +973,7 @@
     </row>
     <row r="18" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B18" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C18" s="1">
         <v>60</v>
@@ -983,27 +983,27 @@
       </c>
       <c r="E18" s="2">
         <f t="shared" si="6"/>
-        <v>130.38</v>
+        <v>124.02000000000001</v>
       </c>
       <c r="F18" s="2">
         <f t="shared" si="7"/>
-        <v>14.486666666666666</v>
+        <v>13.780000000000001</v>
       </c>
       <c r="G18" s="5">
         <f t="shared" si="8"/>
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H18" s="2">
         <f t="shared" si="9"/>
-        <v>65.72</v>
+        <v>62.540000000000006</v>
       </c>
       <c r="I18" s="2">
         <f t="shared" si="10"/>
-        <v>7.3022222222222224</v>
+        <v>6.9488888888888898</v>
       </c>
       <c r="J18" s="5">
         <f t="shared" si="11"/>
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="19" spans="2:10" x14ac:dyDescent="0.35">
@@ -1043,7 +1043,7 @@
     </row>
     <row r="20" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B20" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C20" s="1">
         <v>120</v>
@@ -1053,27 +1053,27 @@
       </c>
       <c r="E20" s="2">
         <f t="shared" si="6"/>
-        <v>260.76</v>
+        <v>248.04000000000002</v>
       </c>
       <c r="F20" s="2">
         <f t="shared" si="7"/>
-        <v>28.973333333333333</v>
+        <v>27.560000000000002</v>
       </c>
       <c r="G20" s="5">
         <f t="shared" si="8"/>
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="H20" s="2">
         <f t="shared" si="9"/>
-        <v>131.44</v>
+        <v>125.08000000000001</v>
       </c>
       <c r="I20" s="2">
         <f t="shared" si="10"/>
-        <v>14.604444444444445</v>
+        <v>13.89777777777778</v>
       </c>
       <c r="J20" s="5">
         <f t="shared" si="11"/>
-        <v>15</v>
+        <v>14</v>
       </c>
     </row>
     <row r="21" spans="2:10" x14ac:dyDescent="0.35">
@@ -1113,7 +1113,7 @@
     </row>
     <row r="22" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B22" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C22" s="1">
         <v>60</v>
@@ -1123,23 +1123,23 @@
       </c>
       <c r="E22" s="2">
         <f t="shared" si="6"/>
-        <v>130.38</v>
+        <v>124.02000000000001</v>
       </c>
       <c r="F22" s="2">
         <f t="shared" si="7"/>
-        <v>14.486666666666666</v>
+        <v>13.780000000000001</v>
       </c>
       <c r="G22" s="5">
         <f t="shared" si="8"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H22" s="2">
         <f t="shared" si="9"/>
-        <v>43.46</v>
+        <v>41.34</v>
       </c>
       <c r="I22" s="2">
         <f t="shared" si="10"/>
-        <v>4.8288888888888888</v>
+        <v>4.5933333333333337</v>
       </c>
       <c r="J22" s="5">
         <f t="shared" si="11"/>
@@ -1183,7 +1183,7 @@
     </row>
     <row r="24" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B24" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C24" s="1">
         <v>120</v>
@@ -1193,23 +1193,23 @@
       </c>
       <c r="E24" s="2">
         <f t="shared" si="6"/>
-        <v>260.76</v>
+        <v>248.04000000000002</v>
       </c>
       <c r="F24" s="2">
         <f t="shared" si="7"/>
-        <v>28.973333333333333</v>
+        <v>27.560000000000002</v>
       </c>
       <c r="G24" s="5">
         <f t="shared" si="8"/>
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="H24" s="2">
         <f t="shared" si="9"/>
-        <v>86.92</v>
+        <v>82.68</v>
       </c>
       <c r="I24" s="2">
         <f t="shared" si="10"/>
-        <v>9.6577777777777776</v>
+        <v>9.1866666666666674</v>
       </c>
       <c r="J24" s="5">
         <f t="shared" si="11"/>
@@ -1253,7 +1253,7 @@
     </row>
     <row r="26" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B26" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C26" s="1">
         <v>60</v>
@@ -1263,23 +1263,23 @@
       </c>
       <c r="E26" s="2">
         <f t="shared" si="6"/>
-        <v>130.38</v>
+        <v>124.02000000000001</v>
       </c>
       <c r="F26" s="2">
         <f t="shared" si="7"/>
-        <v>14.486666666666666</v>
+        <v>13.780000000000001</v>
       </c>
       <c r="G26" s="5">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H26" s="2">
         <f t="shared" si="9"/>
-        <v>32.86</v>
+        <v>31.8</v>
       </c>
       <c r="I26" s="2">
         <f t="shared" si="10"/>
-        <v>3.6511111111111112</v>
+        <v>3.5333333333333332</v>
       </c>
       <c r="J26" s="5">
         <f t="shared" si="11"/>
@@ -1323,7 +1323,7 @@
     </row>
     <row r="28" spans="2:10" x14ac:dyDescent="0.35">
       <c r="B28" s="1">
-        <v>123</v>
+        <v>117</v>
       </c>
       <c r="C28" s="1">
         <v>120</v>
@@ -1333,23 +1333,23 @@
       </c>
       <c r="E28" s="2">
         <f t="shared" si="6"/>
-        <v>260.76</v>
+        <v>248.04000000000002</v>
       </c>
       <c r="F28" s="2">
         <f t="shared" si="7"/>
-        <v>28.973333333333333</v>
+        <v>27.560000000000002</v>
       </c>
       <c r="G28" s="5">
         <f t="shared" si="8"/>
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="H28" s="2">
         <f t="shared" si="9"/>
-        <v>65.72</v>
+        <v>63.6</v>
       </c>
       <c r="I28" s="2">
         <f t="shared" si="10"/>
-        <v>7.3022222222222224</v>
+        <v>7.0666666666666664</v>
       </c>
       <c r="J28" s="5">
         <f t="shared" si="11"/>

</xml_diff>